<commit_message>
creadas las 6 primeras llamadas
</commit_message>
<xml_diff>
--- a/documentacion/peticiones.xlsx
+++ b/documentacion/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="94">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -67,7 +67,7 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
+    <t xml:space="preserve">si</t>
   </si>
   <si>
     <t xml:space="preserve">obtener ultima version</t>
@@ -115,13 +115,16 @@
     <t xml:space="preserve">revisar el archivo de especificaciones para ver exactamente como esta constituido este archivo</t>
   </si>
   <si>
-    <t xml:space="preserve">modificar archivo de configuracion</t>
+    <t xml:space="preserve">crear archivo de configuracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/configuracion</t>
   </si>
   <si>
     <t xml:space="preserve">Sobreescribe un  archivo de configuracion en la version especificada</t>
   </si>
   <si>
-    <t xml:space="preserve">patch</t>
+    <t xml:space="preserve">post</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -139,9 +142,6 @@
   </si>
   <si>
     <t xml:space="preserve">sube un conjunto de datos al servidor especificando la version del archivo de configuracion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">post</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -155,6 +155,9 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">obtener archivo de datos</t>
   </si>
   <si>
@@ -197,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">modifica un objeto en el archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch</t>
   </si>
   <si>
     <t xml:space="preserve">{
@@ -478,8 +484,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -584,7 +590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -606,7 +612,7 @@
       <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -615,25 +621,25 @@
         <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>14</v>
@@ -641,16 +647,16 @@
     </row>
     <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>25</v>
@@ -665,18 +671,18 @@
         <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -685,24 +691,24 @@
         <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -711,30 +717,30 @@
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>38</v>
@@ -743,228 +749,228 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creadas rutas para subir y descargar archivos
</commit_message>
<xml_diff>
--- a/documentacion/peticiones.xlsx
+++ b/documentacion/peticiones.xlsx
@@ -155,9 +155,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">obtener archivo de datos</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
  status: ok, 
 datos: [{objeto_datos}]
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">crear instancia (nueva fila de datos)</t>
@@ -484,8 +484,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -671,18 +671,18 @@
         <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -691,24 +691,24 @@
         <v>25</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -717,10 +717,10 @@
         <v>25</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,7 +749,7 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,7 +757,7 @@
         <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>52</v>
@@ -778,7 +778,7 @@
         <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,7 +804,7 @@
         <v>62</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,7 +830,7 @@
         <v>38</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,7 +854,7 @@
         <v>61</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,7 +880,7 @@
         <v>76</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,7 +901,7 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -924,7 +924,7 @@
         <v>84</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,7 +947,7 @@
         <v>89</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -970,7 +970,7 @@
         <v>93</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminada hasta la llamada 14, postman actualizado, excel actualizado
</commit_message>
<xml_diff>
--- a/documentacion/peticiones.xlsx
+++ b/documentacion/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -179,9 +179,6 @@
 }</t>
   </si>
   <si>
-    <t xml:space="preserve">no</t>
-  </si>
-  <si>
     <t xml:space="preserve">crear instancia (nueva fila de datos)</t>
   </si>
   <si>
@@ -206,7 +203,7 @@
   </si>
   <si>
     <t xml:space="preserve">{
-id: id,
+id: posicion_de_la_instancia,
 objeto: objeto
 }</t>
   </si>
@@ -251,8 +248,15 @@
   </si>
   <si>
     <t xml:space="preserve">{
-nombre_atributo: “nombre”
-}</t>
+atributo: { 
+objeto_configuracion_atributo
+},
+valores:  [{ 
+nombre_atributo: valor 
+}]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisar postman para ver el ejemplo de esta llamada</t>
   </si>
   <si>
     <t xml:space="preserve">eliminar atributo (columna  completa)</t>
@@ -289,6 +293,9 @@
   </si>
   <si>
     <t xml:space="preserve">tener cuidado con no escribir peticiones de borrar o agregar datos, solo solitides de informacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">obtener bases de datos disponibles</t>
@@ -484,8 +491,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -720,18 +727,18 @@
         <v>45</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -740,7 +747,7 @@
         <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>38</v>
@@ -749,73 +756,73 @@
         <v>27</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>31</v>
@@ -824,13 +831,16 @@
         <v>25</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="I13" s="2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,17 +854,17 @@
         <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>70</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,97 +890,97 @@
         <v>76</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creada llamada de archivo de configuracion
</commit_message>
<xml_diff>
--- a/documentacion/peticiones.xlsx
+++ b/documentacion/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="97">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -115,6 +115,29 @@
     <t xml:space="preserve">revisar el archivo de especificaciones para ver exactamente como esta constituido este archivo</t>
   </si>
   <si>
+    <t xml:space="preserve">modificar archivo de configuracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/archivo/?version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifica el archivo tipo configuracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+archivo: {objeto_tipo_configuracion}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+mensaje: “modificado con exito”
+}</t>
+  </si>
+  <si>
     <t xml:space="preserve">crear archivo de configuracion</t>
   </si>
   <si>
@@ -127,18 +150,10 @@
     <t xml:space="preserve">post</t>
   </si>
   <si>
-    <t xml:space="preserve">{
-archivo: {objeto_tipo_configuracion}
-}</t>
-  </si>
-  <si>
     <t xml:space="preserve">revisar el archivo de especificaciones para ver exactamente como esta constituido este archivo, regresa el archivo actualizado</t>
   </si>
   <si>
     <t xml:space="preserve">subir archivo de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/archivo/?version</t>
   </si>
   <si>
     <t xml:space="preserve">sube un conjunto de datos al servidor especificando la version del archivo de configuracion</t>
@@ -199,18 +214,9 @@
     <t xml:space="preserve">modifica un objeto en el archivo</t>
   </si>
   <si>
-    <t xml:space="preserve">patch</t>
-  </si>
-  <si>
     <t xml:space="preserve">{
 id: posicion_de_la_instancia,
 objeto: objeto
-}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
- status: ok, 
-mensaje: “modificado con exito”
 }</t>
   </si>
   <si>
@@ -489,10 +495,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -623,11 +629,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -643,39 +649,36 @@
         <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>14</v>
@@ -686,19 +689,22 @@
         <v>39</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>27</v>
@@ -707,12 +713,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>44</v>
@@ -726,51 +732,48 @@
       <c r="G9" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="I9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="I10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>25</v>
@@ -779,7 +782,7 @@
         <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
@@ -788,199 +791,228 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="I13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="F15" s="5"/>
+      <c r="G15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="I16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>85</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="H17" s="5"/>
       <c r="I17" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>77</v>
+      <c r="C20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>